<commit_message>
Pipeline data now passes initial test_vault_providers test
Drop rows of steel data that are completely empty of data.  This is different than before (where we dropped only columns that were completely empty).

Also update steel input spreadsheet to fix omitted data from Worthington Industries and Carpenter Technology Corp.

Signed-off-by: MichaelTiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/external/mdt-steel-demo.xlsx
+++ b/data/external/mdt-steel-demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/itr-data-pipeline/data/external/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB49987-57FE-CA4B-9ADC-E155C3CDBC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F8381E-E439-3343-9892-C79CBBE0F0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44140" yWindow="25220" windowWidth="43720" windowHeight="21780" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44140" yWindow="25220" windowWidth="43720" windowHeight="21780" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel EI_per_Fe_Ton" sheetId="1" r:id="rId1"/>
@@ -707,10 +707,10 @@
   <dimension ref="A1:AO26"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2098,7 +2098,7 @@
         <v>59</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" ref="E19:G20" si="3">F19</f>
+        <f t="shared" ref="E19:G19" si="3">F19</f>
         <v>0.57634289175025133</v>
       </c>
       <c r="F19" s="2">
@@ -2938,120 +2938,120 @@
         <v>3.4074673629242817E-2</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" ref="L26:T26" si="6">($I26-$U26)*($U$1-L$1)/($U$1-$I$1)+$U26</f>
-        <v>3.4805065445026179E-2</v>
-      </c>
-      <c r="M26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.4194450261780106E-2</v>
-      </c>
-      <c r="N26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.3583835078534033E-2</v>
-      </c>
-      <c r="O26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.297321989528796E-2</v>
-      </c>
-      <c r="P26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.2362604712041887E-2</v>
-      </c>
-      <c r="Q26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.1751989528795814E-2</v>
-      </c>
-      <c r="R26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.1141374345549738E-2</v>
-      </c>
-      <c r="S26" s="2">
-        <f t="shared" si="6"/>
-        <v>3.0530759162303665E-2</v>
-      </c>
-      <c r="T26" s="2">
-        <f t="shared" si="6"/>
-        <v>2.9920143979057592E-2</v>
-      </c>
-      <c r="U26">
-        <f>I26*0.8</f>
-        <v>2.9309528795811519E-2</v>
-      </c>
-      <c r="V26" s="2">
-        <f t="shared" ref="V26:AN26" si="7">($I26-$U26)*($U$1-V$1)/($U$1-$I$1)+$U26</f>
-        <v>2.8698913612565446E-2</v>
-      </c>
-      <c r="W26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.8088298429319373E-2</v>
-      </c>
-      <c r="X26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.74776832460733E-2</v>
-      </c>
-      <c r="Y26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.6867068062827227E-2</v>
-      </c>
-      <c r="Z26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.6256452879581154E-2</v>
-      </c>
-      <c r="AA26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.5645837696335078E-2</v>
-      </c>
-      <c r="AB26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.5035222513089005E-2</v>
-      </c>
-      <c r="AC26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.4424607329842932E-2</v>
-      </c>
-      <c r="AD26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.3813992146596859E-2</v>
-      </c>
-      <c r="AE26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.3203376963350786E-2</v>
-      </c>
-      <c r="AF26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.2592761780104713E-2</v>
-      </c>
-      <c r="AG26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.198214659685864E-2</v>
-      </c>
-      <c r="AH26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.1371531413612567E-2</v>
-      </c>
-      <c r="AI26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.0760916230366494E-2</v>
-      </c>
-      <c r="AJ26" s="2">
-        <f t="shared" si="7"/>
-        <v>2.0150301047120421E-2</v>
-      </c>
-      <c r="AK26" s="2">
-        <f t="shared" si="7"/>
-        <v>1.9539685863874348E-2</v>
-      </c>
-      <c r="AL26" s="2">
-        <f t="shared" si="7"/>
-        <v>1.8929070680628275E-2</v>
-      </c>
-      <c r="AM26" s="2">
-        <f t="shared" si="7"/>
-        <v>1.8318455497382202E-2</v>
-      </c>
-      <c r="AN26" s="2">
-        <f t="shared" si="7"/>
-        <v>1.7707840314136129E-2</v>
+        <f>'Steel CO2e S1'!L26/'Steel Fe_tons'!L28</f>
+        <v>3.1977174821735919E-2</v>
+      </c>
+      <c r="M26" s="10">
+        <f>('Steel CO2e S1'!M26+'Steel CO2e S2'!M26)/'Steel Fe_tons'!M28</f>
+        <v>6.4338890093398632E-2</v>
+      </c>
+      <c r="N26" s="10">
+        <f>('Steel CO2e S1'!N26+'Steel CO2e S2'!N26)/'Steel Fe_tons'!N28</f>
+        <v>6.289692185008823E-2</v>
+      </c>
+      <c r="O26" s="10">
+        <f>('Steel CO2e S1'!O26+'Steel CO2e S2'!O26)/'Steel Fe_tons'!O28</f>
+        <v>6.1483521815409704E-2</v>
+      </c>
+      <c r="P26" s="10">
+        <f>('Steel CO2e S1'!P26+'Steel CO2e S2'!P26)/'Steel Fe_tons'!P28</f>
+        <v>6.0098160533081105E-2</v>
+      </c>
+      <c r="Q26" s="10">
+        <f>('Steel CO2e S1'!Q26+'Steel CO2e S2'!Q26)/'Steel Fe_tons'!Q28</f>
+        <v>5.8740317956509448E-2</v>
+      </c>
+      <c r="R26" s="10">
+        <f>('Steel CO2e S1'!R26+'Steel CO2e S2'!R26)/'Steel Fe_tons'!R28</f>
+        <v>5.7409483286304519E-2</v>
+      </c>
+      <c r="S26" s="10">
+        <f>('Steel CO2e S1'!S26+'Steel CO2e S2'!S26)/'Steel Fe_tons'!S28</f>
+        <v>5.6105154810540132E-2</v>
+      </c>
+      <c r="T26" s="10">
+        <f>('Steel CO2e S1'!T26+'Steel CO2e S2'!T26)/'Steel Fe_tons'!T28</f>
+        <v>5.4826839747717196E-2</v>
+      </c>
+      <c r="U26" s="10">
+        <f>('Steel CO2e S1'!U26+'Steel CO2e S2'!U26)/'Steel Fe_tons'!U28</f>
+        <v>5.35740540923835E-2</v>
+      </c>
+      <c r="V26" s="10">
+        <f>('Steel CO2e S1'!V26+'Steel CO2e S2'!V26)/'Steel Fe_tons'!V28</f>
+        <v>5.0143203337698852E-2</v>
+      </c>
+      <c r="W26" s="10">
+        <f>('Steel CO2e S1'!W26+'Steel CO2e S2'!W26)/'Steel Fe_tons'!W28</f>
+        <v>4.6802056524686518E-2</v>
+      </c>
+      <c r="X26" s="10">
+        <f>('Steel CO2e S1'!X26+'Steel CO2e S2'!X26)/'Steel Fe_tons'!X28</f>
+        <v>4.354871159932517E-2</v>
+      </c>
+      <c r="Y26" s="10">
+        <f>('Steel CO2e S1'!Y26+'Steel CO2e S2'!Y26)/'Steel Fe_tons'!Y28</f>
+        <v>4.0381303134697358E-2</v>
+      </c>
+      <c r="Z26" s="10">
+        <f>('Steel CO2e S1'!Z26+'Steel CO2e S2'!Z26)/'Steel Fe_tons'!Z28</f>
+        <v>3.7298001663821453E-2</v>
+      </c>
+      <c r="AA26" s="10">
+        <f>('Steel CO2e S1'!AA26+'Steel CO2e S2'!AA26)/'Steel Fe_tons'!AA28</f>
+        <v>3.4297013024203647E-2</v>
+      </c>
+      <c r="AB26" s="10">
+        <f>('Steel CO2e S1'!AB26+'Steel CO2e S2'!AB26)/'Steel Fe_tons'!AB28</f>
+        <v>3.1376577713909025E-2</v>
+      </c>
+      <c r="AC26" s="10">
+        <f>('Steel CO2e S1'!AC26+'Steel CO2e S2'!AC26)/'Steel Fe_tons'!AC28</f>
+        <v>2.8534970258954788E-2</v>
+      </c>
+      <c r="AD26" s="10">
+        <f>('Steel CO2e S1'!AD26+'Steel CO2e S2'!AD26)/'Steel Fe_tons'!AD28</f>
+        <v>2.5770498591831097E-2</v>
+      </c>
+      <c r="AE26" s="10">
+        <f>('Steel CO2e S1'!AE26+'Steel CO2e S2'!AE26)/'Steel Fe_tons'!AE28</f>
+        <v>2.3081503440959335E-2</v>
+      </c>
+      <c r="AF26" s="10">
+        <f>('Steel CO2e S1'!AF26+'Steel CO2e S2'!AF26)/'Steel Fe_tons'!AF28</f>
+        <v>2.0466357730899911E-2</v>
+      </c>
+      <c r="AG26" s="10">
+        <f>('Steel CO2e S1'!AG26+'Steel CO2e S2'!AG26)/'Steel Fe_tons'!AG28</f>
+        <v>1.7923465993125266E-2</v>
+      </c>
+      <c r="AH26" s="10">
+        <f>('Steel CO2e S1'!AH26+'Steel CO2e S2'!AH26)/'Steel Fe_tons'!AH28</f>
+        <v>1.5451263787176955E-2</v>
+      </c>
+      <c r="AI26" s="10">
+        <f>('Steel CO2e S1'!AI26+'Steel CO2e S2'!AI26)/'Steel Fe_tons'!AI28</f>
+        <v>1.3048217132028393E-2</v>
+      </c>
+      <c r="AJ26" s="10">
+        <f>('Steel CO2e S1'!AJ26+'Steel CO2e S2'!AJ26)/'Steel Fe_tons'!AJ28</f>
+        <v>1.0712821947478158E-2</v>
+      </c>
+      <c r="AK26" s="10">
+        <f>('Steel CO2e S1'!AK26+'Steel CO2e S2'!AK26)/'Steel Fe_tons'!AK28</f>
+        <v>8.4436035054015045E-3</v>
+      </c>
+      <c r="AL26" s="10">
+        <f>('Steel CO2e S1'!AL26+'Steel CO2e S2'!AL26)/'Steel Fe_tons'!AL28</f>
+        <v>6.2391158906907667E-3</v>
+      </c>
+      <c r="AM26" s="10">
+        <f>('Steel CO2e S1'!AM26+'Steel CO2e S2'!AM26)/'Steel Fe_tons'!AM28</f>
+        <v>4.0979414717180742E-3</v>
+      </c>
+      <c r="AN26" s="10">
+        <f>('Steel CO2e S1'!AN26+'Steel CO2e S2'!AN26)/'Steel Fe_tons'!AN28</f>
+        <v>2.0186903801566874E-3</v>
       </c>
       <c r="AO26">
         <v>0</v>
@@ -3072,10 +3072,10 @@
   <dimension ref="A1:AO28"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="M28" sqref="M28:AO28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3566,7 +3566,7 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E2:G6" si="3">F4</f>
+        <f t="shared" ref="E4:G6" si="3">F4</f>
         <v>138831</v>
       </c>
       <c r="F4">
@@ -3633,7 +3633,7 @@
         <v>163535.82892825236</v>
       </c>
       <c r="V4" s="2">
-        <f t="shared" ref="V2:AE6" si="5">$U4*1.015^(V$1-$U$1)</f>
+        <f t="shared" ref="V4:AE6" si="5">$U4*1.015^(V$1-$U$1)</f>
         <v>165988.86636217614</v>
       </c>
       <c r="W4" s="2">
@@ -3673,7 +3673,7 @@
         <v>189790.00582556555</v>
       </c>
       <c r="AF4" s="2">
-        <f t="shared" ref="AF2:AO6" si="6">$U4*1.015^(AF$1-$U$1)</f>
+        <f t="shared" ref="AF4:AO6" si="6">$U4*1.015^(AF$1-$U$1)</f>
         <v>192636.85591294902</v>
       </c>
       <c r="AG4" s="2">
@@ -5080,19 +5080,19 @@
         <v>65</v>
       </c>
       <c r="E23" s="2">
-        <f>F23</f>
+        <f t="shared" ref="E23:H24" si="20">F23</f>
         <v>10953432.098765431</v>
       </c>
       <c r="F23" s="2">
-        <f>G23</f>
+        <f t="shared" si="20"/>
         <v>10953432.098765431</v>
       </c>
       <c r="G23" s="2">
-        <f>H23</f>
+        <f t="shared" si="20"/>
         <v>10953432.098765431</v>
       </c>
       <c r="H23">
-        <f>I23</f>
+        <f t="shared" si="20"/>
         <v>10953432.098765431</v>
       </c>
       <c r="I23" s="11">
@@ -5176,55 +5176,55 @@
         <v>13462668.646640068</v>
       </c>
       <c r="AC23" s="2">
-        <f t="shared" ref="AC23:AO24" si="20">$J23*1.015^(AC$1-$J$1)</f>
+        <f t="shared" ref="AC23:AO24" si="21">$J23*1.015^(AC$1-$J$1)</f>
         <v>13664608.676339667</v>
       </c>
       <c r="AD23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>13869577.806484759</v>
       </c>
       <c r="AE23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>14077621.473582029</v>
       </c>
       <c r="AF23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>14288785.795685757</v>
       </c>
       <c r="AG23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>14503117.582621042</v>
       </c>
       <c r="AH23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>14720664.346360356</v>
       </c>
       <c r="AI23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>14941474.31155576</v>
       </c>
       <c r="AJ23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>15165596.426229093</v>
       </c>
       <c r="AK23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>15393080.372622529</v>
       </c>
       <c r="AL23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>15623976.578211863</v>
       </c>
       <c r="AM23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>15858336.226885041</v>
       </c>
       <c r="AN23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>16096211.270288311</v>
       </c>
       <c r="AO23" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>16337654.439342635</v>
       </c>
     </row>
@@ -5239,19 +5239,19 @@
         <v>68</v>
       </c>
       <c r="E24" s="2">
-        <f>F24</f>
+        <f t="shared" si="20"/>
         <v>1472468.75</v>
       </c>
       <c r="F24" s="2">
-        <f>G24</f>
+        <f t="shared" si="20"/>
         <v>1472468.75</v>
       </c>
       <c r="G24" s="2">
-        <f>H24</f>
+        <f t="shared" si="20"/>
         <v>1472468.75</v>
       </c>
       <c r="H24" s="2">
-        <f>I24</f>
+        <f t="shared" si="20"/>
         <v>1472468.75</v>
       </c>
       <c r="I24" s="14">
@@ -5335,55 +5335,55 @@
         <v>1760865.2732811347</v>
       </c>
       <c r="AC24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1787278.2523803515</v>
       </c>
       <c r="AD24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1814087.4261660562</v>
       </c>
       <c r="AE24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1841298.7375585469</v>
       </c>
       <c r="AF24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1868918.2186219248</v>
       </c>
       <c r="AG24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1896951.9919012536</v>
       </c>
       <c r="AH24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1925406.2717797719</v>
       </c>
       <c r="AI24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1954287.3658564684</v>
       </c>
       <c r="AJ24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1983601.6763443153</v>
       </c>
       <c r="AK24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2013355.7014894797</v>
       </c>
       <c r="AL24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2043556.0370118213</v>
       </c>
       <c r="AM24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2074209.3775669988</v>
       </c>
       <c r="AN24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2105322.518230503</v>
       </c>
       <c r="AO24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2136902.3560039606</v>
       </c>
     </row>
@@ -5434,119 +5434,119 @@
         <v>13547990.508045182</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" ref="M26:U26" si="21">$H26*1.015^(M$1-$H$1)</f>
+        <f t="shared" ref="M26:U28" si="22">$H26*1.015^(M$1-$H$1)</f>
         <v>15555981.016090365</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>15789320.731331717</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>16026160.54230169</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>16266552.950436214</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>16510551.244692756</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>16758209.513363145</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>17009582.65606359</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>17264726.395904541</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>17523697.291843109</v>
       </c>
       <c r="V26" s="2">
-        <f t="shared" ref="V26:AO26" si="22">$U26*1.015^(V$1-$U$1)</f>
+        <f t="shared" ref="V26:AO26" si="23">$U26*1.015^(V$1-$U$1)</f>
         <v>17786552.751220755</v>
       </c>
       <c r="W26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>18053351.042489063</v>
       </c>
       <c r="X26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>18324151.308126397</v>
       </c>
       <c r="Y26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>18599013.577748287</v>
       </c>
       <c r="Z26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>18877998.781414513</v>
       </c>
       <c r="AA26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>19161168.763135724</v>
       </c>
       <c r="AB26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>19448586.294582758</v>
       </c>
       <c r="AC26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>19740315.089001499</v>
       </c>
       <c r="AD26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>20036419.815336518</v>
       </c>
       <c r="AE26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>20336966.112566564</v>
       </c>
       <c r="AF26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>20642020.604255058</v>
       </c>
       <c r="AG26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>20951650.91331888</v>
       </c>
       <c r="AH26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>21265925.677018661</v>
       </c>
       <c r="AI26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>21584914.562173937</v>
       </c>
       <c r="AJ26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>21908688.280606542</v>
       </c>
       <c r="AK26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>22237318.60481564</v>
       </c>
       <c r="AL26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>22570878.383887868</v>
       </c>
       <c r="AM26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>22909441.559646185</v>
       </c>
       <c r="AN26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>23253083.183040876</v>
       </c>
       <c r="AO26" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>23601879.430786483</v>
       </c>
     </row>
@@ -5594,6 +5594,122 @@
       </c>
       <c r="L28">
         <v>4067000</v>
+      </c>
+      <c r="M28" s="2">
+        <f>$L28*1.015^(M$1-$L$1)</f>
+        <v>4128004.9999999995</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" ref="N28:AO28" si="24">$L28*1.015^(N$1-$L$1)</f>
+        <v>4189925.0749999988</v>
+      </c>
+      <c r="O28" s="2">
+        <f t="shared" si="24"/>
+        <v>4252773.9511249987</v>
+      </c>
+      <c r="P28" s="2">
+        <f t="shared" si="24"/>
+        <v>4316565.5603918731</v>
+      </c>
+      <c r="Q28" s="2">
+        <f t="shared" si="24"/>
+        <v>4381314.04379775</v>
+      </c>
+      <c r="R28" s="2">
+        <f t="shared" si="24"/>
+        <v>4447033.7544547152</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="24"/>
+        <v>4513739.2607715353</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="24"/>
+        <v>4581445.3496831087</v>
+      </c>
+      <c r="U28" s="2">
+        <f t="shared" si="24"/>
+        <v>4650167.0299283545</v>
+      </c>
+      <c r="V28" s="2">
+        <f t="shared" si="24"/>
+        <v>4719919.5353772789</v>
+      </c>
+      <c r="W28" s="2">
+        <f t="shared" si="24"/>
+        <v>4790718.3284079377</v>
+      </c>
+      <c r="X28" s="2">
+        <f t="shared" si="24"/>
+        <v>4862579.1033340562</v>
+      </c>
+      <c r="Y28" s="2">
+        <f t="shared" si="24"/>
+        <v>4935517.7898840662</v>
+      </c>
+      <c r="Z28" s="2">
+        <f t="shared" si="24"/>
+        <v>5009550.5567323258</v>
+      </c>
+      <c r="AA28" s="2">
+        <f t="shared" si="24"/>
+        <v>5084693.81508331</v>
+      </c>
+      <c r="AB28" s="2">
+        <f t="shared" si="24"/>
+        <v>5160964.2223095596</v>
+      </c>
+      <c r="AC28" s="2">
+        <f t="shared" si="24"/>
+        <v>5238378.6856442019</v>
+      </c>
+      <c r="AD28" s="2">
+        <f t="shared" si="24"/>
+        <v>5316954.3659288641</v>
+      </c>
+      <c r="AE28" s="2">
+        <f t="shared" si="24"/>
+        <v>5396708.6814177968</v>
+      </c>
+      <c r="AF28" s="2">
+        <f t="shared" si="24"/>
+        <v>5477659.3116390621</v>
+      </c>
+      <c r="AG28" s="2">
+        <f t="shared" si="24"/>
+        <v>5559824.2013136474</v>
+      </c>
+      <c r="AH28" s="2">
+        <f t="shared" si="24"/>
+        <v>5643221.5643333513</v>
+      </c>
+      <c r="AI28" s="2">
+        <f t="shared" si="24"/>
+        <v>5727869.8877983512</v>
+      </c>
+      <c r="AJ28" s="2">
+        <f t="shared" si="24"/>
+        <v>5813787.9361153254</v>
+      </c>
+      <c r="AK28" s="2">
+        <f t="shared" si="24"/>
+        <v>5900994.7551570553</v>
+      </c>
+      <c r="AL28" s="2">
+        <f t="shared" si="24"/>
+        <v>5989509.6764844097</v>
+      </c>
+      <c r="AM28" s="2">
+        <f t="shared" si="24"/>
+        <v>6079352.3216316756</v>
+      </c>
+      <c r="AN28" s="2">
+        <f t="shared" si="24"/>
+        <v>6170542.6064561494</v>
+      </c>
+      <c r="AO28" s="2">
+        <f t="shared" si="24"/>
+        <v>6263100.7455529915</v>
       </c>
     </row>
   </sheetData>
@@ -5610,11 +5726,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5854,6 +5970,10 @@
         <f>'Steel EI_per_Fe_Ton'!T2*'Steel Fe_tons'!T4</f>
         <v>234322.73895678335</v>
       </c>
+      <c r="U2" s="2">
+        <f>'Steel EI_per_Fe_Ton'!U2*'Steel Fe_tons'!U4</f>
+        <v>226511.98099155718</v>
+      </c>
       <c r="V2">
         <f>'Steel EI_per_Fe_Ton'!V2*'Steel Fe_tons'!V4</f>
         <v>218414.17767110901</v>
@@ -6665,7 +6785,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16:I16" si="9">F16</f>
+        <f t="shared" ref="E16:H16" si="9">F16</f>
         <v>4800000</v>
       </c>
       <c r="F16" s="2">
@@ -7142,19 +7262,19 @@
         <v>62</v>
       </c>
       <c r="E20" s="2">
-        <f>F20</f>
+        <f t="shared" ref="E20:H22" si="15">F20</f>
         <v>2000000</v>
       </c>
       <c r="F20" s="2">
-        <f>G20</f>
+        <f t="shared" si="15"/>
         <v>2000000</v>
       </c>
       <c r="G20" s="2">
-        <f>H20</f>
+        <f t="shared" si="15"/>
         <v>2000000</v>
       </c>
       <c r="H20">
-        <f>I20</f>
+        <f t="shared" si="15"/>
         <v>2000000</v>
       </c>
       <c r="I20" s="6">
@@ -7174,31 +7294,31 @@
         <v>1844444.4444444445</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" ref="N20:T20" si="15">($L20-$U20)*($U$1-N$1)/($U$1-$L$1)+$U20</f>
+        <f t="shared" ref="N20:T20" si="16">($L20-$U20)*($U$1-N$1)/($U$1-$L$1)+$U20</f>
         <v>1788888.888888889</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1733333.3333333333</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1677777.7777777778</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1622222.2222222222</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1566666.6666666667</v>
       </c>
       <c r="S20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1511111.111111111</v>
       </c>
       <c r="T20" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1455555.5555555555</v>
       </c>
       <c r="U20" s="6">
@@ -7296,19 +7416,19 @@
         <v>65</v>
       </c>
       <c r="E21" s="5">
-        <f>F21</f>
+        <f t="shared" si="15"/>
         <v>17744560</v>
       </c>
       <c r="F21" s="5">
-        <f>G21</f>
+        <f t="shared" si="15"/>
         <v>17744560</v>
       </c>
       <c r="G21" s="5">
-        <f>H21</f>
+        <f t="shared" si="15"/>
         <v>17744560</v>
       </c>
       <c r="H21" s="5">
-        <f>I21</f>
+        <f t="shared" si="15"/>
         <v>17744560</v>
       </c>
       <c r="I21" s="8">
@@ -7321,39 +7441,39 @@
         <v>15257923</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" ref="L21:T24" si="16">($K21-$U21)*($U$1-L$1)/($U$1-$K$1)+$U21</f>
+        <f t="shared" ref="L21:T24" si="17">($K21-$U21)*($U$1-L$1)/($U$1-$K$1)+$U21</f>
         <v>15151695.5</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>15045468</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14939240.5</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14833013</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14726785.5</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14620558</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14514330.5</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14408103</v>
       </c>
       <c r="T21" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>14301875.5</v>
       </c>
       <c r="U21" s="6">
@@ -7451,19 +7571,19 @@
         <v>68</v>
       </c>
       <c r="E22" s="5">
-        <f>F22</f>
+        <f t="shared" si="15"/>
         <v>99660</v>
       </c>
       <c r="F22" s="5">
-        <f>G22</f>
+        <f t="shared" si="15"/>
         <v>99660</v>
       </c>
       <c r="G22" s="5">
-        <f>H22</f>
+        <f t="shared" si="15"/>
         <v>99660</v>
       </c>
       <c r="H22" s="5">
-        <f>I22</f>
+        <f t="shared" si="15"/>
         <v>99660</v>
       </c>
       <c r="I22" s="13">
@@ -7476,39 +7596,39 @@
         <v>91490</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>88320.6</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>85151.2</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>81981.8</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>78812.399999999994</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>75643</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>72473.600000000006</v>
       </c>
       <c r="R22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>69304.2</v>
       </c>
       <c r="S22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>66134.8</v>
       </c>
       <c r="T22" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>62965.4</v>
       </c>
       <c r="U22" s="6">
@@ -7645,39 +7765,39 @@
         <v>24500000</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>24650000</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>24800000</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>24950000</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25100000</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25250000</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25400000</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25550000</v>
       </c>
       <c r="S24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25700000</v>
       </c>
       <c r="T24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25850000</v>
       </c>
       <c r="U24" s="6">
@@ -7814,39 +7934,39 @@
         <v>130506</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" ref="L26:T26" si="17">($K26-$U26)*($U$1-L$1)/($U$1-$K$1)+$U26</f>
+        <f t="shared" ref="L26:T26" si="18">($K26-$U26)*($U$1-L$1)/($U$1-$K$1)+$U26</f>
         <v>130051.17</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>129596.34</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>129141.51</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>128686.68</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>128231.85</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>127777.02</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>127322.19</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>126867.36</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>126412.53</v>
       </c>
       <c r="U26" s="11">
@@ -7854,79 +7974,79 @@
         <v>125957.7</v>
       </c>
       <c r="V26" s="2">
-        <f t="shared" ref="V26:AN26" si="18">$U26*($AO$1-V$1)/($AO$1-$U$1)</f>
+        <f t="shared" ref="V26:AN26" si="19">$U26*($AO$1-V$1)/($AO$1-$U$1)</f>
         <v>119659.81499999999</v>
       </c>
       <c r="W26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>113361.93000000001</v>
       </c>
       <c r="X26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>107064.045</v>
       </c>
       <c r="Y26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>100766.16</v>
       </c>
       <c r="Z26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>94468.274999999994</v>
       </c>
       <c r="AA26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>88170.39</v>
       </c>
       <c r="AB26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>81872.50499999999</v>
       </c>
       <c r="AC26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>75574.62</v>
       </c>
       <c r="AD26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>69276.735000000001</v>
       </c>
       <c r="AE26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>62978.85</v>
       </c>
       <c r="AF26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>56680.965000000004</v>
       </c>
       <c r="AG26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>50383.08</v>
       </c>
       <c r="AH26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>44085.195</v>
       </c>
       <c r="AI26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>37787.31</v>
       </c>
       <c r="AJ26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>31489.424999999999</v>
       </c>
       <c r="AK26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>25191.54</v>
       </c>
       <c r="AL26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>18893.654999999999</v>
       </c>
       <c r="AM26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>12595.77</v>
       </c>
       <c r="AN26" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>6297.8850000000002</v>
       </c>
       <c r="AO26" s="2">
@@ -7947,7 +8067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFF0462-5620-5640-A6FC-BB7C149CC476}">
   <dimension ref="A1:AO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -9008,7 +9128,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16:I16" si="10">F16</f>
+        <f t="shared" ref="E16:H16" si="10">F16</f>
         <v>5785714.2857142854</v>
       </c>
       <c r="F16" s="2">
@@ -9487,19 +9607,19 @@
         <v>62</v>
       </c>
       <c r="E20" s="2">
-        <f>F20</f>
+        <f t="shared" ref="E20:H22" si="17">F20</f>
         <v>1000000</v>
       </c>
       <c r="F20" s="2">
-        <f>G20</f>
+        <f t="shared" si="17"/>
         <v>1000000</v>
       </c>
       <c r="G20" s="2">
-        <f>H20</f>
+        <f t="shared" si="17"/>
         <v>1000000</v>
       </c>
       <c r="H20" s="2">
-        <f>I20</f>
+        <f t="shared" si="17"/>
         <v>1000000</v>
       </c>
       <c r="I20" s="6">
@@ -9519,31 +9639,31 @@
         <v>788888.88888888888</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" ref="N20:T20" si="17">($L20-$U20)*($U$1-N$1)/($U$1-$L$1)+$U20</f>
+        <f t="shared" ref="N20:T20" si="18">($L20-$U20)*($U$1-N$1)/($U$1-$L$1)+$U20</f>
         <v>777777.77777777775</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>766666.66666666663</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>755555.5555555555</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>744444.4444444445</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>733333.33333333337</v>
       </c>
       <c r="S20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>722222.22222222225</v>
       </c>
       <c r="T20" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>711111.11111111112</v>
       </c>
       <c r="U20" s="6">
@@ -9641,19 +9761,19 @@
         <v>65</v>
       </c>
       <c r="E21" s="5">
-        <f>F21</f>
+        <f t="shared" si="17"/>
         <v>858941</v>
       </c>
       <c r="F21" s="5">
-        <f>G21</f>
+        <f t="shared" si="17"/>
         <v>858941</v>
       </c>
       <c r="G21" s="5">
-        <f>H21</f>
+        <f t="shared" si="17"/>
         <v>858941</v>
       </c>
       <c r="H21" s="5">
-        <f>I21</f>
+        <f t="shared" si="17"/>
         <v>858941</v>
       </c>
       <c r="I21" s="8">
@@ -9666,39 +9786,39 @@
         <v>1154111</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" ref="L21:T22" si="18">($K21-$U21)*($U$1-L$1)/($U$1-$K$1)+$U21</f>
+        <f t="shared" ref="L21:T22" si="19">($K21-$U21)*($U$1-L$1)/($U$1-$K$1)+$U21</f>
         <v>1107415.1800000002</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1060719.3599999999</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1014023.54</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>967327.72</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>920631.9</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>873936.08000000007</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>827240.26</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>780544.44000000006</v>
       </c>
       <c r="T21" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>733848.62</v>
       </c>
       <c r="U21" s="6">
@@ -9796,19 +9916,19 @@
         <v>68</v>
       </c>
       <c r="E22" s="5">
-        <f>F22</f>
+        <f t="shared" si="17"/>
         <v>371530</v>
       </c>
       <c r="F22" s="5">
-        <f>G22</f>
+        <f t="shared" si="17"/>
         <v>371530</v>
       </c>
       <c r="G22" s="5">
-        <f>H22</f>
+        <f t="shared" si="17"/>
         <v>371530</v>
       </c>
       <c r="H22" s="5">
-        <f>I22</f>
+        <f t="shared" si="17"/>
         <v>371530</v>
       </c>
       <c r="I22" s="13">
@@ -9821,39 +9941,39 @@
         <v>316640</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>307267.8</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>297895.59999999998</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>288523.40000000002</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>279151.2</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>269779</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>260406.8</v>
       </c>
       <c r="R22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>251034.6</v>
       </c>
       <c r="S22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>241662.4</v>
       </c>
       <c r="T22" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>232290.2</v>
       </c>
       <c r="U22" s="6">
@@ -9986,39 +10106,39 @@
         <v>2000000</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" ref="L24:T26" si="19">($K24-$U24)*($U$1-L$1)/($U$1-$K$1)+$U24</f>
+        <f t="shared" ref="L24:T26" si="20">($K24-$U24)*($U$1-L$1)/($U$1-$K$1)+$U24</f>
         <v>2064000</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2128000</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2192000</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2256000</v>
       </c>
       <c r="P24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2320000</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2384000</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2448000</v>
       </c>
       <c r="S24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2512000</v>
       </c>
       <c r="T24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2576000</v>
       </c>
       <c r="U24" s="6">
@@ -10026,79 +10146,79 @@
         <v>2640000</v>
       </c>
       <c r="V24" s="2">
-        <f t="shared" ref="V24:AN26" si="20">$U24*($AO$1-V$1)/($AO$1-$U$1)</f>
+        <f t="shared" ref="V24:AN26" si="21">$U24*($AO$1-V$1)/($AO$1-$U$1)</f>
         <v>2508000</v>
       </c>
       <c r="W24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2376000</v>
       </c>
       <c r="X24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2244000</v>
       </c>
       <c r="Y24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2112000</v>
       </c>
       <c r="Z24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1980000</v>
       </c>
       <c r="AA24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1848000</v>
       </c>
       <c r="AB24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1716000</v>
       </c>
       <c r="AC24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1584000</v>
       </c>
       <c r="AD24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1452000</v>
       </c>
       <c r="AE24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1320000</v>
       </c>
       <c r="AF24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1188000</v>
       </c>
       <c r="AG24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1056000</v>
       </c>
       <c r="AH24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>924000</v>
       </c>
       <c r="AI24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>792000</v>
       </c>
       <c r="AJ24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>660000</v>
       </c>
       <c r="AK24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>528000</v>
       </c>
       <c r="AL24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>396000</v>
       </c>
       <c r="AM24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>264000</v>
       </c>
       <c r="AN24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>132000</v>
       </c>
       <c r="AO24" s="2">
@@ -10155,39 +10275,39 @@
         <v>139201</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>137597.96</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>135994.91999999998</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>134391.88</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>132788.84</v>
       </c>
       <c r="P26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>131185.79999999999</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>129582.76</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>127979.72</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>126376.68</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>124773.63999999998</v>
       </c>
       <c r="U26" s="11">
@@ -10195,79 +10315,79 @@
         <v>123170.59999999999</v>
       </c>
       <c r="V26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>117012.06999999999</v>
       </c>
       <c r="W26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>110853.54</v>
       </c>
       <c r="X26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>104695.01</v>
       </c>
       <c r="Y26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>98536.48</v>
       </c>
       <c r="Z26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>92377.949999999983</v>
       </c>
       <c r="AA26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>86219.42</v>
       </c>
       <c r="AB26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>80060.889999999985</v>
       </c>
       <c r="AC26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>73902.36</v>
       </c>
       <c r="AD26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>67743.829999999987</v>
       </c>
       <c r="AE26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>61585.3</v>
       </c>
       <c r="AF26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>55426.77</v>
       </c>
       <c r="AG26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>49268.24</v>
       </c>
       <c r="AH26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>43109.71</v>
       </c>
       <c r="AI26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>36951.18</v>
       </c>
       <c r="AJ26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>30792.65</v>
       </c>
       <c r="AK26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>24634.12</v>
       </c>
       <c r="AL26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>18475.59</v>
       </c>
       <c r="AM26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>12317.06</v>
       </c>
       <c r="AN26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>6158.53</v>
       </c>
       <c r="AO26" s="2">
@@ -10916,7 +11036,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E15:I18" si="5">F16</f>
+        <f t="shared" ref="E16:H16" si="5">F16</f>
         <v>7557446.8085106378</v>
       </c>
       <c r="F16" s="2">
@@ -11250,19 +11370,19 @@
         <v>62</v>
       </c>
       <c r="E20" s="2">
-        <f>F20</f>
+        <f t="shared" ref="E20:H21" si="11">F20</f>
         <v>3200000</v>
       </c>
       <c r="F20" s="2">
-        <f>G20</f>
+        <f t="shared" si="11"/>
         <v>3200000</v>
       </c>
       <c r="G20" s="2">
-        <f>H20</f>
+        <f t="shared" si="11"/>
         <v>3200000</v>
       </c>
       <c r="H20" s="2">
-        <f>I20</f>
+        <f t="shared" si="11"/>
         <v>3200000</v>
       </c>
       <c r="I20" s="6">
@@ -11278,35 +11398,35 @@
         <v>1700000</v>
       </c>
       <c r="M20" s="11">
-        <f t="shared" ref="M20:T20" si="11">($J20-$U20)*($U$1-M$1)/($U$1-$J$1)+$U20</f>
+        <f t="shared" ref="M20:T20" si="12">($J20-$U20)*($U$1-M$1)/($U$1-$J$1)+$U20</f>
         <v>2111818.1818181816</v>
       </c>
       <c r="N20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2049090.9090909092</v>
       </c>
       <c r="O20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1986363.6363636362</v>
       </c>
       <c r="P20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1923636.3636363638</v>
       </c>
       <c r="Q20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1860909.0909090908</v>
       </c>
       <c r="R20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1798181.8181818181</v>
       </c>
       <c r="S20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1735454.5454545454</v>
       </c>
       <c r="T20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1672727.2727272727</v>
       </c>
       <c r="U20" s="11">
@@ -11314,79 +11434,79 @@
         <v>1610000</v>
       </c>
       <c r="V20" s="2">
-        <f t="shared" ref="V20:AN21" si="12">$U20*($AO$1-V$1)/($AO$1-$U$1)</f>
+        <f t="shared" ref="V20:AN21" si="13">$U20*($AO$1-V$1)/($AO$1-$U$1)</f>
         <v>1529500</v>
       </c>
       <c r="W20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1449000</v>
       </c>
       <c r="X20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1368500</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1288000</v>
       </c>
       <c r="Z20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1207500</v>
       </c>
       <c r="AA20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1127000</v>
       </c>
       <c r="AB20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1046500</v>
       </c>
       <c r="AC20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>966000</v>
       </c>
       <c r="AD20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>885500</v>
       </c>
       <c r="AE20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>805000</v>
       </c>
       <c r="AF20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>724500</v>
       </c>
       <c r="AG20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>644000</v>
       </c>
       <c r="AH20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>563500</v>
       </c>
       <c r="AI20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>483000</v>
       </c>
       <c r="AJ20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>402500</v>
       </c>
       <c r="AK20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>322000</v>
       </c>
       <c r="AL20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>241500</v>
       </c>
       <c r="AM20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>161000</v>
       </c>
       <c r="AN20" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>80500</v>
       </c>
       <c r="AO20" s="2">
@@ -11404,19 +11524,19 @@
         <v>65</v>
       </c>
       <c r="E21" s="5">
-        <f>F21</f>
+        <f t="shared" si="11"/>
         <v>1056210</v>
       </c>
       <c r="F21" s="5">
-        <f>G21</f>
+        <f t="shared" si="11"/>
         <v>1056210</v>
       </c>
       <c r="G21" s="5">
-        <f>H21</f>
+        <f t="shared" si="11"/>
         <v>1056210</v>
       </c>
       <c r="H21" s="5">
-        <f>I21</f>
+        <f t="shared" si="11"/>
         <v>1056210</v>
       </c>
       <c r="I21" s="8">
@@ -11429,39 +11549,39 @@
         <v>767666</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" ref="L21:T21" si="13">($K21-$U21)*($U$1-L$1)/($U$1-$K$1)+$U21</f>
+        <f t="shared" ref="L21:T21" si="14">($K21-$U21)*($U$1-L$1)/($U$1-$K$1)+$U21</f>
         <v>764834.1</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>762002.2</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>759170.3</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>756338.4</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>753506.5</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>750674.6</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>747842.7</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>745010.8</v>
       </c>
       <c r="T21" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>742178.9</v>
       </c>
       <c r="U21" s="11">
@@ -11469,79 +11589,79 @@
         <v>739347</v>
       </c>
       <c r="V21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>702379.65</v>
       </c>
       <c r="W21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>665412.30000000005</v>
       </c>
       <c r="X21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>628444.94999999995</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>591477.6</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>554510.25</v>
       </c>
       <c r="AA21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>517542.9</v>
       </c>
       <c r="AB21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>480575.55</v>
       </c>
       <c r="AC21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>443608.2</v>
       </c>
       <c r="AD21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>406640.85</v>
       </c>
       <c r="AE21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>369673.5</v>
       </c>
       <c r="AF21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>332706.15000000002</v>
       </c>
       <c r="AG21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>295738.8</v>
       </c>
       <c r="AH21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>258771.45</v>
       </c>
       <c r="AI21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>221804.1</v>
       </c>
       <c r="AJ21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>184836.75</v>
       </c>
       <c r="AK21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>147869.4</v>
       </c>
       <c r="AL21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>110902.05</v>
       </c>
       <c r="AM21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>73934.7</v>
       </c>
       <c r="AN21" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36967.35</v>
       </c>
       <c r="AO21" s="2">

</xml_diff>